<commit_message>
Update on 20250829 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/移动直播源/海南移动/海南移动可用IP和可看频道列表.xlsx
+++ b/直播源汇总文档/移动直播源/海南移动/海南移动可用IP和可看频道列表.xlsx
@@ -12,15 +12,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hainan_Mobile_V4!$A$1:$A$5071</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hainan_Mobile_V6!$A$1:$A$781</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hainan_Mobile_V4!$A$1:$A$5084</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hainan_Mobile_V6!$A$1:$A$783</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5852" uniqueCount="5852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5867" uniqueCount="5867">
   <si>
     <t>CCTV-1,http://[2409:8087:5e08:25::4]:6610/000000001000/5000000004000002226/1.m3u8?IAS$海南移动V6</t>
   </si>
@@ -17582,6 +17582,51 @@
   </si>
   <si>
     <t>NEWTV精品纪录,http://39.134.136.205:6610/200000001898/460000089800010076/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://[2409:8087:5e08:25::4]:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V6</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://[2409:8087:5e08:25::16]:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V6</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.196:6410/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.197:6410/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.198:6410/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.196:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.197:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.198:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.199:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.200:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.201:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.202:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.203:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.204:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
+  </si>
+  <si>
+    <t>NEWTV武搏世界,http://39.134.136.205:6610/000000001000/bokesen/1.m3u8?IAS$海南移动V4</t>
   </si>
 </sst>
 </file>
@@ -17932,7 +17977,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A781"/>
+  <dimension ref="A1:A783"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21748,106 +21793,116 @@
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A762" t="s">
-        <v>4941</v>
+        <v>5852</v>
       </c>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A763" t="s">
-        <v>4942</v>
+        <v>5853</v>
       </c>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A764" t="s">
-        <v>4943</v>
+        <v>4941</v>
       </c>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A765" t="s">
-        <v>4944</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="766" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A766" t="s">
-        <v>4945</v>
+        <v>4943</v>
       </c>
     </row>
     <row r="767" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A767" t="s">
-        <v>4946</v>
+        <v>4944</v>
       </c>
     </row>
     <row r="768" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A768" t="s">
-        <v>4947</v>
+        <v>4945</v>
       </c>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A769" t="s">
-        <v>4948</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A770" t="s">
-        <v>4949</v>
+        <v>4947</v>
       </c>
     </row>
     <row r="771" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A771" t="s">
-        <v>4950</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A772" t="s">
-        <v>4951</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A773" t="s">
-        <v>4952</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="774" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A774" t="s">
-        <v>640</v>
+        <v>4951</v>
       </c>
     </row>
     <row r="775" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A775" t="s">
-        <v>641</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="776" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A776" t="s">
-        <v>472</v>
+        <v>640</v>
       </c>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A777" t="s">
-        <v>473</v>
+        <v>641</v>
       </c>
     </row>
     <row r="778" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A778" t="s">
-        <v>631</v>
+        <v>472</v>
       </c>
     </row>
     <row r="779" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A779" t="s">
-        <v>632</v>
+        <v>473</v>
       </c>
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A780" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
     </row>
     <row r="781" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A781" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A782" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A783" t="s">
         <v>639</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A781"/>
+  <autoFilter ref="A1:A783"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21855,7 +21910,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5071"/>
+  <dimension ref="A1:A5084"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -46571,656 +46626,721 @@
     </row>
     <row r="4942" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4942" t="s">
-        <v>5759</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="4943" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4943" t="s">
-        <v>5760</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="4944" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4944" t="s">
-        <v>5761</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="4945" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4945" t="s">
-        <v>5762</v>
+        <v>5857</v>
       </c>
     </row>
     <row r="4946" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4946" t="s">
-        <v>5763</v>
+        <v>5858</v>
       </c>
     </row>
     <row r="4947" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4947" t="s">
-        <v>5764</v>
+        <v>5859</v>
       </c>
     </row>
     <row r="4948" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4948" t="s">
-        <v>5765</v>
+        <v>5860</v>
       </c>
     </row>
     <row r="4949" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4949" t="s">
-        <v>5766</v>
+        <v>5861</v>
       </c>
     </row>
     <row r="4950" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4950" t="s">
-        <v>5767</v>
+        <v>5862</v>
       </c>
     </row>
     <row r="4951" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4951" t="s">
-        <v>5768</v>
+        <v>5863</v>
       </c>
     </row>
     <row r="4952" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4952" t="s">
-        <v>5769</v>
+        <v>5864</v>
       </c>
     </row>
     <row r="4953" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4953" t="s">
-        <v>5770</v>
+        <v>5865</v>
       </c>
     </row>
     <row r="4954" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4954" t="s">
-        <v>5771</v>
+        <v>5866</v>
       </c>
     </row>
     <row r="4955" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4955" t="s">
-        <v>5772</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="4956" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4956" t="s">
-        <v>5773</v>
+        <v>5760</v>
       </c>
     </row>
     <row r="4957" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4957" t="s">
-        <v>5774</v>
+        <v>5761</v>
       </c>
     </row>
     <row r="4958" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4958" t="s">
-        <v>5775</v>
+        <v>5762</v>
       </c>
     </row>
     <row r="4959" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4959" t="s">
-        <v>5776</v>
+        <v>5763</v>
       </c>
     </row>
     <row r="4960" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4960" t="s">
-        <v>5777</v>
+        <v>5764</v>
       </c>
     </row>
     <row r="4961" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4961" t="s">
-        <v>5778</v>
+        <v>5765</v>
       </c>
     </row>
     <row r="4962" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4962" t="s">
-        <v>5779</v>
+        <v>5766</v>
       </c>
     </row>
     <row r="4963" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4963" t="s">
-        <v>5780</v>
+        <v>5767</v>
       </c>
     </row>
     <row r="4964" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4964" t="s">
-        <v>5781</v>
+        <v>5768</v>
       </c>
     </row>
     <row r="4965" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4965" t="s">
-        <v>5782</v>
+        <v>5769</v>
       </c>
     </row>
     <row r="4966" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4966" t="s">
-        <v>5783</v>
+        <v>5770</v>
       </c>
     </row>
     <row r="4967" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4967" t="s">
-        <v>5784</v>
+        <v>5771</v>
       </c>
     </row>
     <row r="4968" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4968" t="s">
-        <v>5785</v>
+        <v>5772</v>
       </c>
     </row>
     <row r="4969" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4969" t="s">
-        <v>5786</v>
+        <v>5773</v>
       </c>
     </row>
     <row r="4970" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4970" t="s">
-        <v>5787</v>
+        <v>5774</v>
       </c>
     </row>
     <row r="4971" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4971" t="s">
-        <v>5788</v>
+        <v>5775</v>
       </c>
     </row>
     <row r="4972" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4972" t="s">
-        <v>5789</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="4973" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4973" t="s">
-        <v>5790</v>
+        <v>5777</v>
       </c>
     </row>
     <row r="4974" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4974" t="s">
-        <v>5791</v>
+        <v>5778</v>
       </c>
     </row>
     <row r="4975" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4975" t="s">
-        <v>5792</v>
+        <v>5779</v>
       </c>
     </row>
     <row r="4976" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4976" t="s">
-        <v>5793</v>
+        <v>5780</v>
       </c>
     </row>
     <row r="4977" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4977" t="s">
-        <v>5794</v>
+        <v>5781</v>
       </c>
     </row>
     <row r="4978" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4978" t="s">
-        <v>5795</v>
+        <v>5782</v>
       </c>
     </row>
     <row r="4979" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4979" t="s">
-        <v>5796</v>
+        <v>5783</v>
       </c>
     </row>
     <row r="4980" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4980" t="s">
-        <v>5797</v>
+        <v>5784</v>
       </c>
     </row>
     <row r="4981" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4981" t="s">
-        <v>5798</v>
+        <v>5785</v>
       </c>
     </row>
     <row r="4982" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4982" t="s">
-        <v>5799</v>
+        <v>5786</v>
       </c>
     </row>
     <row r="4983" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4983" t="s">
-        <v>5800</v>
+        <v>5787</v>
       </c>
     </row>
     <row r="4984" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4984" t="s">
-        <v>5801</v>
+        <v>5788</v>
       </c>
     </row>
     <row r="4985" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4985" t="s">
-        <v>5802</v>
+        <v>5789</v>
       </c>
     </row>
     <row r="4986" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4986" t="s">
-        <v>5803</v>
+        <v>5790</v>
       </c>
     </row>
     <row r="4987" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4987" t="s">
-        <v>5804</v>
+        <v>5791</v>
       </c>
     </row>
     <row r="4988" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4988" t="s">
-        <v>5805</v>
+        <v>5792</v>
       </c>
     </row>
     <row r="4989" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4989" t="s">
-        <v>5806</v>
+        <v>5793</v>
       </c>
     </row>
     <row r="4990" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4990" t="s">
-        <v>5807</v>
+        <v>5794</v>
       </c>
     </row>
     <row r="4991" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4991" t="s">
-        <v>5808</v>
+        <v>5795</v>
       </c>
     </row>
     <row r="4992" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4992" t="s">
-        <v>5809</v>
+        <v>5796</v>
       </c>
     </row>
     <row r="4993" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4993" t="s">
-        <v>5810</v>
+        <v>5797</v>
       </c>
     </row>
     <row r="4994" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4994" t="s">
-        <v>5811</v>
+        <v>5798</v>
       </c>
     </row>
     <row r="4995" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4995" t="s">
-        <v>5812</v>
+        <v>5799</v>
       </c>
     </row>
     <row r="4996" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4996" t="s">
-        <v>5813</v>
+        <v>5800</v>
       </c>
     </row>
     <row r="4997" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4997" t="s">
-        <v>5814</v>
+        <v>5801</v>
       </c>
     </row>
     <row r="4998" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4998" t="s">
-        <v>5815</v>
+        <v>5802</v>
       </c>
     </row>
     <row r="4999" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4999" t="s">
-        <v>5816</v>
+        <v>5803</v>
       </c>
     </row>
     <row r="5000" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5000" t="s">
-        <v>5817</v>
+        <v>5804</v>
       </c>
     </row>
     <row r="5001" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5001" t="s">
-        <v>5818</v>
+        <v>5805</v>
       </c>
     </row>
     <row r="5002" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5002" t="s">
-        <v>5819</v>
+        <v>5806</v>
       </c>
     </row>
     <row r="5003" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5003" t="s">
-        <v>5820</v>
+        <v>5807</v>
       </c>
     </row>
     <row r="5004" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5004" t="s">
-        <v>5821</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="5005" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5005" t="s">
-        <v>5822</v>
+        <v>5809</v>
       </c>
     </row>
     <row r="5006" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5006" t="s">
-        <v>5823</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="5007" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5007" t="s">
-        <v>5824</v>
+        <v>5811</v>
       </c>
     </row>
     <row r="5008" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5008" t="s">
-        <v>5825</v>
+        <v>5812</v>
       </c>
     </row>
     <row r="5009" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5009" t="s">
-        <v>5826</v>
+        <v>5813</v>
       </c>
     </row>
     <row r="5010" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5010" t="s">
-        <v>5827</v>
+        <v>5814</v>
       </c>
     </row>
     <row r="5011" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5011" t="s">
-        <v>5828</v>
+        <v>5815</v>
       </c>
     </row>
     <row r="5012" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5012" t="s">
-        <v>5829</v>
+        <v>5816</v>
       </c>
     </row>
     <row r="5013" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5013" t="s">
-        <v>5830</v>
+        <v>5817</v>
       </c>
     </row>
     <row r="5014" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5014" t="s">
-        <v>5831</v>
+        <v>5818</v>
       </c>
     </row>
     <row r="5015" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5015" t="s">
-        <v>5832</v>
+        <v>5819</v>
       </c>
     </row>
     <row r="5016" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5016" t="s">
-        <v>5833</v>
+        <v>5820</v>
       </c>
     </row>
     <row r="5017" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5017" t="s">
-        <v>5834</v>
+        <v>5821</v>
       </c>
     </row>
     <row r="5018" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5018" t="s">
-        <v>5835</v>
+        <v>5822</v>
       </c>
     </row>
     <row r="5019" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5019" t="s">
-        <v>5836</v>
+        <v>5823</v>
       </c>
     </row>
     <row r="5020" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5020" t="s">
-        <v>4765</v>
+        <v>5824</v>
       </c>
     </row>
     <row r="5021" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5021" t="s">
-        <v>4766</v>
+        <v>5825</v>
       </c>
     </row>
     <row r="5022" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5022" t="s">
-        <v>4767</v>
+        <v>5826</v>
       </c>
     </row>
     <row r="5023" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5023" t="s">
-        <v>4768</v>
+        <v>5827</v>
       </c>
     </row>
     <row r="5024" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5024" t="s">
-        <v>4769</v>
+        <v>5828</v>
       </c>
     </row>
     <row r="5025" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5025" t="s">
-        <v>4770</v>
+        <v>5829</v>
       </c>
     </row>
     <row r="5026" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5026" t="s">
-        <v>4771</v>
+        <v>5830</v>
       </c>
     </row>
     <row r="5027" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5027" t="s">
-        <v>4772</v>
+        <v>5831</v>
       </c>
     </row>
     <row r="5028" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5028" t="s">
-        <v>4773</v>
+        <v>5832</v>
       </c>
     </row>
     <row r="5029" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5029" t="s">
-        <v>4774</v>
+        <v>5833</v>
       </c>
     </row>
     <row r="5030" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5030" t="s">
-        <v>4775</v>
+        <v>5834</v>
       </c>
     </row>
     <row r="5031" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5031" t="s">
-        <v>4776</v>
+        <v>5835</v>
       </c>
     </row>
     <row r="5032" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5032" t="s">
-        <v>4777</v>
+        <v>5836</v>
       </c>
     </row>
     <row r="5033" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5033" t="s">
-        <v>4778</v>
+        <v>4765</v>
       </c>
     </row>
     <row r="5034" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5034" t="s">
-        <v>4779</v>
+        <v>4766</v>
       </c>
     </row>
     <row r="5035" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5035" t="s">
-        <v>4780</v>
+        <v>4767</v>
       </c>
     </row>
     <row r="5036" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5036" t="s">
-        <v>4781</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="5037" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5037" t="s">
-        <v>4782</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="5038" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5038" t="s">
-        <v>4783</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="5039" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5039" t="s">
-        <v>4784</v>
+        <v>4771</v>
       </c>
     </row>
     <row r="5040" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5040" t="s">
-        <v>4785</v>
+        <v>4772</v>
       </c>
     </row>
     <row r="5041" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5041" t="s">
-        <v>4786</v>
+        <v>4773</v>
       </c>
     </row>
     <row r="5042" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5042" t="s">
-        <v>4787</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="5043" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5043" t="s">
-        <v>4788</v>
+        <v>4775</v>
       </c>
     </row>
     <row r="5044" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5044" t="s">
-        <v>4789</v>
+        <v>4776</v>
       </c>
     </row>
     <row r="5045" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5045" t="s">
-        <v>4790</v>
+        <v>4777</v>
       </c>
     </row>
     <row r="5046" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5046" t="s">
-        <v>4791</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="5047" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5047" t="s">
-        <v>4792</v>
+        <v>4779</v>
       </c>
     </row>
     <row r="5048" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5048" t="s">
-        <v>4793</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="5049" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5049" t="s">
-        <v>4794</v>
+        <v>4781</v>
       </c>
     </row>
     <row r="5050" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5050" t="s">
-        <v>4795</v>
+        <v>4782</v>
       </c>
     </row>
     <row r="5051" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5051" t="s">
-        <v>4796</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="5052" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5052" t="s">
-        <v>4797</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="5053" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5053" t="s">
-        <v>4798</v>
+        <v>4785</v>
       </c>
     </row>
     <row r="5054" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5054" t="s">
-        <v>4799</v>
+        <v>4786</v>
       </c>
     </row>
     <row r="5055" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5055" t="s">
-        <v>4800</v>
+        <v>4787</v>
       </c>
     </row>
     <row r="5056" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5056" t="s">
-        <v>4801</v>
+        <v>4788</v>
       </c>
     </row>
     <row r="5057" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5057" t="s">
-        <v>4802</v>
+        <v>4789</v>
       </c>
     </row>
     <row r="5058" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5058" t="s">
-        <v>4803</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="5059" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5059" t="s">
-        <v>4804</v>
+        <v>4791</v>
       </c>
     </row>
     <row r="5060" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5060" t="s">
-        <v>4805</v>
+        <v>4792</v>
       </c>
     </row>
     <row r="5061" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5061" t="s">
-        <v>4806</v>
+        <v>4793</v>
       </c>
     </row>
     <row r="5062" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5062" t="s">
-        <v>4807</v>
+        <v>4794</v>
       </c>
     </row>
     <row r="5063" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5063" t="s">
-        <v>4808</v>
+        <v>4795</v>
       </c>
     </row>
     <row r="5064" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5064" t="s">
-        <v>4809</v>
+        <v>4796</v>
       </c>
     </row>
     <row r="5065" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5065" t="s">
-        <v>4810</v>
+        <v>4797</v>
       </c>
     </row>
     <row r="5066" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5066" t="s">
-        <v>4811</v>
+        <v>4798</v>
       </c>
     </row>
     <row r="5067" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5067" t="s">
-        <v>4812</v>
+        <v>4799</v>
       </c>
     </row>
     <row r="5068" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5068" t="s">
-        <v>4813</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="5069" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5069" t="s">
-        <v>4814</v>
+        <v>4801</v>
       </c>
     </row>
     <row r="5070" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5070" t="s">
-        <v>4815</v>
+        <v>4802</v>
       </c>
     </row>
     <row r="5071" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5071" t="s">
+        <v>4803</v>
+      </c>
+    </row>
+    <row r="5072" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5072" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="5073" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5073" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="5074" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5074" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="5075" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5075" t="s">
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="5076" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5076" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="5077" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5077" t="s">
+        <v>4809</v>
+      </c>
+    </row>
+    <row r="5078" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5078" t="s">
+        <v>4810</v>
+      </c>
+    </row>
+    <row r="5079" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5079" t="s">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="5080" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5080" t="s">
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="5081" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5081" t="s">
+        <v>4813</v>
+      </c>
+    </row>
+    <row r="5082" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5082" t="s">
+        <v>4814</v>
+      </c>
+    </row>
+    <row r="5083" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5083" t="s">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="5084" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5084" t="s">
         <v>4816</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A5071"/>
+  <autoFilter ref="A1:A5084"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>